<commit_message>
Correction engine motor + overflow bottles
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F9CC7F-AA9E-4C0D-B381-28F45D912526}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="3036" windowWidth="17280" windowHeight="8028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="3036" windowWidth="17280" windowHeight="8028"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>System</t>
   </si>
@@ -222,11 +221,17 @@
   <si>
     <t>Fuel injectors</t>
   </si>
+  <si>
+    <t>Second-hand, PC40</t>
+  </si>
+  <si>
+    <t>From PC37, outlet at the opposite of PC40 version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,21 +646,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="70.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
@@ -709,7 +714,9 @@
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
@@ -777,7 +784,9 @@
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
@@ -918,7 +927,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -937,7 +946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -971,7 +980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -990,7 +999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">

</xml_diff>

<commit_message>
Correction EN + oublie soufflets steering
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911EC3C4-DCE7-4186-B774-9D5870C19027}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>System</t>
   </si>
@@ -139,9 +138,6 @@
     <t xml:space="preserve">Contain engine's oil </t>
   </si>
   <si>
-    <t>Permit to limit the oil displacement in the oil sump</t>
-  </si>
-  <si>
     <t>Oil overflow</t>
   </si>
   <si>
@@ -190,12 +186,6 @@
     <t>Shifter axis</t>
   </si>
   <si>
-    <t>Permit to adjust the speed rotation between the shifter axis and the gear box selector</t>
-  </si>
-  <si>
-    <t>Permit to transmit the rotation of the gear motor into the gear box selector</t>
-  </si>
-  <si>
     <t>EN_01013</t>
   </si>
   <si>
@@ -205,18 +195,12 @@
     <t>Join plate</t>
   </si>
   <si>
-    <t>Permit to attach the oil system to the engine</t>
-  </si>
-  <si>
     <t>Fuel injectors</t>
   </si>
   <si>
     <t>Second-hand, PC40</t>
   </si>
   <si>
-    <t>From PC37, outlet at the opposite of PC40 version</t>
-  </si>
-  <si>
     <t>Smooth clutch disc</t>
   </si>
   <si>
@@ -224,12 +208,24 @@
   </si>
   <si>
     <t>Discs of the clutch system</t>
+  </si>
+  <si>
+    <t>From PC37</t>
+  </si>
+  <si>
+    <t>Attach the oil sump shell to the engine</t>
+  </si>
+  <si>
+    <t>Limit oil displacement in the oil sump</t>
+  </si>
+  <si>
+    <t>Shaft between Shifter and gear motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,15 +672,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
@@ -745,7 +741,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -758,7 +754,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>21</v>
@@ -775,7 +771,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>21</v>
@@ -792,7 +788,7 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
@@ -809,13 +805,13 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -859,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -878,71 +874,71 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F13" s="4">
         <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>21</v>
@@ -952,45 +948,43 @@
         <v>7</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1012,13 +1006,13 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -1031,13 +1025,13 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
DESO MAJ DBOM ENGINE
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D64E68-C00F-4BA1-9611-ADED7E99725D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F53DAC3-1894-41F3-B210-7A4E3BF29420}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,22 @@
     <sheet name="EN_A0100" sheetId="2" r:id="rId2"/>
     <sheet name="EN_A0800" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="105">
   <si>
     <t>System</t>
   </si>
@@ -243,18 +248,12 @@
     <t>To be completed</t>
   </si>
   <si>
-    <t>Tba</t>
-  </si>
-  <si>
     <t>Process</t>
   </si>
   <si>
     <t>Fasteners</t>
   </si>
   <si>
-    <t>Tooling</t>
-  </si>
-  <si>
     <t>EN - Engine assembly</t>
   </si>
   <si>
@@ -267,9 +266,6 @@
     <t>EN_A0800_P</t>
   </si>
   <si>
-    <t>Screw M10x80</t>
-  </si>
-  <si>
     <t>PAIR Plate</t>
   </si>
   <si>
@@ -282,9 +278,6 @@
     <t>Laser cut</t>
   </si>
   <si>
-    <t>Screw M4x8</t>
-  </si>
-  <si>
     <t>Sheet 2,5mm</t>
   </si>
   <si>
@@ -300,9 +293,6 @@
     <t>Sheet 8mm</t>
   </si>
   <si>
-    <t>Water cut</t>
-  </si>
-  <si>
     <t>Welded to Oil sump shell</t>
   </si>
   <si>
@@ -327,9 +317,6 @@
     <t>Shifter Gear</t>
   </si>
   <si>
-    <t>Screw M10x160</t>
-  </si>
-  <si>
     <t>Steel 30NCD6</t>
   </si>
   <si>
@@ -349,6 +336,42 @@
   </si>
   <si>
     <t>Aluminium 2017A</t>
+  </si>
+  <si>
+    <t>Install Tie wrap</t>
+  </si>
+  <si>
+    <t>Machining (conventionnal)</t>
+  </si>
+  <si>
+    <t>Tighten bolt</t>
+  </si>
+  <si>
+    <t>Fastener install</t>
+  </si>
+  <si>
+    <t>Bolt grade 8,8 M10</t>
+  </si>
+  <si>
+    <t>Bolt grade 8,8 M8</t>
+  </si>
+  <si>
+    <t>Bolt grade 8,8 M4</t>
+  </si>
+  <si>
+    <t>Washer M10</t>
+  </si>
+  <si>
+    <t>Washer M8</t>
+  </si>
+  <si>
+    <t>Washer M4</t>
+  </si>
+  <si>
+    <t>Water jet cut</t>
+  </si>
+  <si>
+    <t>Machining (CNC)</t>
   </si>
 </sst>
 </file>
@@ -580,16 +603,16 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -948,8 +971,8 @@
       <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>87</v>
+      <c r="H3" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -968,8 +991,8 @@
       <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>87</v>
+      <c r="H4" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -988,8 +1011,8 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>87</v>
+      <c r="H5" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1008,8 +1031,8 @@
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>87</v>
+      <c r="H6" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1030,8 +1053,8 @@
       <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>87</v>
+      <c r="H7" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1052,8 +1075,8 @@
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>88</v>
+      <c r="H8" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1074,8 +1097,8 @@
       <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>87</v>
+      <c r="H9" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1096,8 +1119,8 @@
       <c r="G10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>88</v>
+      <c r="H10" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1118,8 +1141,8 @@
       <c r="G11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>88</v>
+      <c r="H11" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1140,8 +1163,8 @@
       <c r="G12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>88</v>
+      <c r="H12" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1153,7 +1176,7 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="4">
@@ -1162,8 +1185,8 @@
       <c r="G13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>87</v>
+      <c r="H13" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1175,15 +1198,15 @@
       <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="4">
         <v>7</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>87</v>
+      <c r="H14" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1204,8 +1227,8 @@
       <c r="G15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>87</v>
+      <c r="H15" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1224,8 +1247,8 @@
       <c r="G16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>87</v>
+      <c r="H16" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1292,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,9 +1327,9 @@
     <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1338,7 +1361,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1363,7 +1386,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1371,13 +1394,13 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G4" s="8">
         <v>2</v>
@@ -1389,13 +1412,13 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -1407,13 +1430,13 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G6" s="8">
         <v>8</v>
@@ -1425,13 +1448,13 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G7" s="8">
         <v>4</v>
@@ -1442,53 +1465,63 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8">
+        <v>2</v>
+      </c>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <v>4</v>
+      </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>13</v>
-      </c>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>74</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11" s="7"/>
     </row>
@@ -1497,64 +1530,64 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>15</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="G15" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -1563,66 +1596,64 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>81</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F19" s="8"/>
       <c r="G19" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -1631,14 +1662,14 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -1647,68 +1678,66 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G21" s="8">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="8">
         <v>2</v>
       </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="11">
-        <v>1</v>
-      </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F24" s="8"/>
       <c r="G24" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="7"/>
     </row>
@@ -1717,14 +1746,16 @@
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="G25" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="7"/>
     </row>
@@ -1733,15 +1764,15 @@
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="8">
+        <v>80</v>
+      </c>
+      <c r="G26" s="9">
         <v>1</v>
       </c>
       <c r="H26" s="7"/>
@@ -1749,7 +1780,7 @@
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>21</v>
@@ -1759,7 +1790,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1770,9 +1801,11 @@
         <v>61</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="G28" s="8">
         <v>1</v>
       </c>
@@ -1783,11 +1816,15 @@
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="G29" s="8">
+        <v>1</v>
+      </c>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1795,17 +1832,23 @@
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="8">
+        <v>1</v>
+      </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>21</v>
@@ -1815,7 +1858,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1826,7 +1869,7 @@
         <v>61</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8">
@@ -1839,80 +1882,120 @@
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="6" t="s">
+    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6" t="s">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F36" s="8"/>
-      <c r="G36" s="8">
-        <v>1</v>
-      </c>
+      <c r="G36" s="8"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
+    <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="8">
+        <v>1</v>
+      </c>
       <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1922,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1967,7 +2050,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1985,14 +2068,14 @@
         <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2000,284 +2083,18 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>63</v>
+      <c r="G4" s="8">
+        <v>8</v>
       </c>
       <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAJ BOM EN 2
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA41527-336A-4E8F-A0A1-01A45BDDB852}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBECD72-AA7B-483D-9E18-703918D4C204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="115">
   <si>
     <t>System</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Put the shifter axis inside the engine</t>
   </si>
   <si>
-    <t>Put the shifter gear on the shifter axis</t>
-  </si>
-  <si>
     <t>Instal the wet slipper clutch</t>
   </si>
   <si>
@@ -396,6 +393,15 @@
   </si>
   <si>
     <t>Permit to lock the shifter axis inside the engine</t>
+  </si>
+  <si>
+    <t>Bolt grade 8.8 M8x40</t>
+  </si>
+  <si>
+    <t>Bolt between shifter gear and the engine mecanism</t>
+  </si>
+  <si>
+    <t>Permit to lock gear on the engine</t>
   </si>
 </sst>
 </file>
@@ -1339,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1352,7 +1358,7 @@
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" customWidth="1"/>
     <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" customWidth="1"/>
   </cols>
@@ -1658,16 +1664,16 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G18" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -1676,13 +1682,13 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G19" s="8">
         <v>2</v>
@@ -1694,16 +1700,16 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G20" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -1718,7 +1724,7 @@
         <v>105</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G21" s="8">
         <v>1</v>
@@ -1733,129 +1739,131 @@
         <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="8">
-        <v>1</v>
-      </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="F23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G26" s="8">
         <v>2</v>
       </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8">
-        <v>2</v>
-      </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>73</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F27" s="8"/>
       <c r="G27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8">
-        <v>1</v>
-      </c>
-      <c r="H28" s="7"/>
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="G29" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H29" s="7"/>
     </row>
@@ -1867,78 +1875,76 @@
         <v>63</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>76</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="8">
         <v>1</v>
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6" t="s">
-        <v>33</v>
-      </c>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8">
+        <v>4</v>
+      </c>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G32" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8">
-        <v>2</v>
-      </c>
-      <c r="H33" s="7"/>
+    <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G34" s="8">
         <v>2</v>
@@ -1952,220 +1958,254 @@
       <c r="D35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G35" s="9">
-        <v>1</v>
+      <c r="E35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8">
+        <v>2</v>
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6" t="s">
-        <v>38</v>
-      </c>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="8">
+        <v>2</v>
+      </c>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="8">
+        <v>80</v>
+      </c>
+      <c r="G37" s="9">
         <v>1</v>
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8">
-        <v>1</v>
-      </c>
-      <c r="H38" s="7"/>
+    <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="8">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" s="8">
-        <v>1</v>
-      </c>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="E40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="8">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8">
-        <v>1</v>
-      </c>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8">
+        <v>1</v>
+      </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8">
-        <v>1</v>
-      </c>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8">
-        <v>1</v>
-      </c>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7" t="s">
+      <c r="F49" s="8"/>
+      <c r="G49" s="8">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="7"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAJ BOM EN 3
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0100_ENA0800.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\CR - Cost Report\BOM\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBECD72-AA7B-483D-9E18-703918D4C204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971F0C91-63C6-483B-B9AC-8035D7607F69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
   <si>
     <t>System</t>
   </si>
@@ -402,6 +402,21 @@
   </si>
   <si>
     <t>Permit to lock gear on the engine</t>
+  </si>
+  <si>
+    <t>Center bolt to lock the clutch inside the engine</t>
+  </si>
+  <si>
+    <t>Bolt M12</t>
+  </si>
+  <si>
+    <t>Bolt M6</t>
+  </si>
+  <si>
+    <t>To contraint the clutch mecanism</t>
+  </si>
+  <si>
+    <t>To lock the top of the thermostat on the thermostat</t>
   </si>
 </sst>
 </file>
@@ -929,22 +944,22 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="53.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +983,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -983,7 +998,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1005,7 +1020,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -1025,7 +1040,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -1045,7 +1060,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -1065,7 +1080,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1087,7 +1102,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -1109,7 +1124,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -1131,7 +1146,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
@@ -1153,7 +1168,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1175,7 +1190,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -1197,7 +1212,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -1219,7 +1234,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -1239,7 +1254,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -1261,7 +1276,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -1281,7 +1296,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -1315,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
@@ -1345,25 +1360,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
@@ -1403,7 +1418,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>60</v>
@@ -1419,7 +1434,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1437,7 +1452,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1455,7 +1470,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1473,7 +1488,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1491,7 +1506,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1509,7 +1524,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1527,7 +1542,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1543,7 +1558,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1559,7 +1574,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1575,7 +1590,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1591,7 +1606,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1607,7 +1622,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1623,7 +1638,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1641,7 +1656,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1659,7 +1674,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1677,7 +1692,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1695,7 +1710,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1713,7 +1728,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1731,7 +1746,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1747,7 +1762,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1765,7 +1780,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1783,7 +1798,7 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>69</v>
@@ -1799,7 +1814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1817,7 +1832,7 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1833,7 +1848,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>25</v>
@@ -1849,7 +1864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1867,7 +1882,7 @@
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1883,7 +1898,7 @@
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1899,7 +1914,7 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1917,7 +1932,7 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6" t="s">
         <v>89</v>
@@ -1933,7 +1948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1951,7 +1966,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1967,7 +1982,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1985,7 +2000,7 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2003,7 +2018,7 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6" t="s">
         <v>81</v>
@@ -2019,7 +2034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2037,7 +2052,7 @@
       </c>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2053,7 +2068,7 @@
       </c>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2071,7 +2086,7 @@
       </c>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
         <v>84</v>
@@ -2087,7 +2102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2103,7 +2118,7 @@
       </c>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2117,7 +2132,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
         <v>85</v>
@@ -2133,7 +2148,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2149,7 +2164,7 @@
       </c>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2163,7 +2178,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
         <v>23</v>
@@ -2179,7 +2194,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2195,7 +2210,7 @@
       </c>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2206,6 +2221,92 @@
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G52" s="8">
+        <v>1</v>
+      </c>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G53" s="8">
+        <v>6</v>
+      </c>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G55" s="8">
+        <v>2</v>
+      </c>
+      <c r="H55" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2221,18 +2322,18 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
@@ -2272,7 +2373,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>60</v>
@@ -2288,7 +2389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>

</xml_diff>